<commit_message>
Adding spreadsheet for all runs
</commit_message>
<xml_diff>
--- a/source/MySEProject/Documentation/experiment-run.xlsx
+++ b/source/MySEProject/Documentation/experiment-run.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a76e50f64a8dee0b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dea28d49ea53da6a/Study/Sem I/SE/project/neocortexapi/source/MySEProject/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A856EBFD-BC6D-4B5E-932D-AAB24D3C2492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A856EBFD-BC6D-4B5E-932D-AAB24D3C2492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6FB3EA1-69D5-400E-8867-B1457FE7A883}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02780977-10FF-4881-9E68-23A93F5DC7D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02780977-10FF-4881-9E68-23A93F5DC7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>No. of runs</t>
   </si>
   <si>
     <t>max accuracy</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -1480,20 +1483,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4F5128-900D-4D3D-A790-DE4840198503}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B41" sqref="A1:B41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>54.16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>20.83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>83.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>58.33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>54.16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>54.16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>58.33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>54.66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>45.83</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1813,12 +1816,21 @@
         <v>41.66</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <f>AVERAGE(B2:B41)</f>
+        <v>47.686750000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>